<commit_message>
add Lok Fu normal Photos
</commit_message>
<xml_diff>
--- a/Estates Progress.xlsx
+++ b/Estates Progress.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="101">
   <si>
     <t>Region</t>
   </si>
@@ -328,10 +328,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -354,14 +362,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -643,7 +654,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1296,11 +1307,11 @@
       <c r="K20" t="s">
         <v>84</v>
       </c>
-      <c r="L20" t="s">
-        <v>95</v>
+      <c r="L20" s="1">
+        <v>43978</v>
       </c>
       <c r="M20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -1325,14 +1336,14 @@
       <c r="J21">
         <v>11</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="L21" t="s">
-        <v>95</v>
+      <c r="L21" s="1">
+        <v>43978</v>
       </c>
       <c r="M21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
@@ -1360,11 +1371,11 @@
       <c r="K22" t="s">
         <v>90</v>
       </c>
-      <c r="L22" t="s">
-        <v>95</v>
+      <c r="L22" s="1">
+        <v>43978</v>
       </c>
       <c r="M22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -1400,7 +1411,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K21" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>